<commit_message>
Results from June 11, 2020 12:01 AM run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-06-10.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-06-10.xlsx
@@ -365,7 +365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,48 +423,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>North Carolina</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>43992</v>
+      </c>
+      <c r="C2" t="n">
+        <v>21626</v>
+      </c>
+      <c r="D2" t="n">
+        <v>739</v>
+      </c>
+      <c r="E2" t="n">
+        <v>9221</v>
+      </c>
+      <c r="F2" t="n">
+        <v>333</v>
+      </c>
+      <c r="G2" t="n">
+        <v>42.64</v>
+      </c>
+      <c r="H2" t="n">
+        <v>45.06</v>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>An error occurred. ... ValueError('Unable to extract date from table header.')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wisconsin -- Milwaukee</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="C3" t="n">
-        <v>9001</v>
+        <v>593</v>
       </c>
       <c r="D3" t="n">
-        <v>301</v>
+        <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>2571</v>
+        <v>16</v>
       </c>
       <c r="F3" t="n">
-        <v>129</v>
-      </c>
-      <c r="G3" t="n">
-        <v>28.56</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1.43</v>
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -475,48 +493,74 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Michigan</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>43991</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>97336</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4600</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>4713</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>9.8</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>An error occurred. ... UnboundLocalError("local variable 'date_published' referenced before assignment")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>California - San Diego</t>
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>43991</v>
+        <v>43991.99836937636</v>
       </c>
       <c r="C5" t="n">
-        <v>103889</v>
+        <v>8729</v>
       </c>
       <c r="D5" t="n">
-        <v>7408</v>
+        <v>301</v>
       </c>
       <c r="E5" t="n">
-        <v>9652</v>
+        <v>260</v>
       </c>
       <c r="F5" t="n">
-        <v>617</v>
+        <v>9</v>
       </c>
       <c r="G5" t="n">
-        <v>9.289999999999999</v>
+        <v>2.98</v>
       </c>
       <c r="H5" t="n">
-        <v>8.33</v>
+        <v>2.99</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -527,29 +571,29 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Texas -- Bexar County</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="C6" t="n">
-        <v>1805</v>
+        <v>28499</v>
       </c>
       <c r="D6" t="n">
-        <v>54</v>
+        <v>1573</v>
       </c>
       <c r="E6" t="n">
-        <v>276</v>
+        <v>1676</v>
       </c>
       <c r="F6" t="n">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="G6" t="n">
-        <v>15.29</v>
+        <v>5.88</v>
       </c>
       <c r="H6" t="n">
-        <v>31.48</v>
+        <v>6.74</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -560,29 +604,31 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Minnesota</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>43991</v>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2020-06-10</t>
+        </is>
       </c>
       <c r="C7" t="n">
-        <v>28523</v>
+        <v>65779</v>
       </c>
       <c r="D7" t="n">
-        <v>1217</v>
+        <v>2801</v>
       </c>
       <c r="E7" t="n">
-        <v>6283</v>
+        <v>12198</v>
       </c>
       <c r="F7" t="n">
-        <v>78</v>
+        <v>558</v>
       </c>
       <c r="G7" t="n">
-        <v>22.03</v>
+        <v>18.54</v>
       </c>
       <c r="H7" t="n">
-        <v>6.41</v>
+        <v>19.92</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -593,31 +639,29 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Florida</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2020-06-09</t>
-        </is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>43992</v>
       </c>
       <c r="C8" t="n">
-        <v>64448</v>
+        <v>53980</v>
       </c>
       <c r="D8" t="n">
-        <v>2765</v>
+        <v>2329</v>
       </c>
       <c r="E8" t="n">
-        <v>11954</v>
+        <v>16965</v>
       </c>
       <c r="F8" t="n">
-        <v>551</v>
+        <v>1123</v>
       </c>
       <c r="G8" t="n">
-        <v>18.55</v>
+        <v>31.43</v>
       </c>
       <c r="H8" t="n">
-        <v>19.93</v>
+        <v>48.22</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -628,29 +672,29 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B9" s="3" t="n">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="C9" t="n">
-        <v>9474</v>
+        <v>104156</v>
       </c>
       <c r="D9" t="n">
-        <v>495</v>
+        <v>7454</v>
       </c>
       <c r="E9" t="n">
-        <v>4331</v>
+        <v>9729</v>
       </c>
       <c r="F9" t="n">
-        <v>367</v>
+        <v>620</v>
       </c>
       <c r="G9" t="n">
-        <v>45.71</v>
+        <v>9.34</v>
       </c>
       <c r="H9" t="n">
-        <v>74.14</v>
+        <v>8.32</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -661,62 +705,48 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>California - San Diego</t>
-        </is>
-      </c>
-      <c r="B10" s="3" t="n">
-        <v>43991.01301612313</v>
-      </c>
-      <c r="C10" t="n">
-        <v>8729</v>
-      </c>
-      <c r="D10" t="n">
-        <v>301</v>
-      </c>
-      <c r="E10" t="n">
-        <v>260</v>
-      </c>
-      <c r="F10" t="n">
-        <v>9</v>
-      </c>
-      <c r="G10" t="n">
-        <v>2.98</v>
-      </c>
-      <c r="H10" t="n">
-        <v>2.99</v>
-      </c>
+          <t>Michigan</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... UnboundLocalError("local variable 'date_published' referenced before assignment")</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="C11" t="n">
-        <v>53249</v>
+        <v>28869</v>
       </c>
       <c r="D11" t="n">
-        <v>2285</v>
+        <v>1236</v>
       </c>
       <c r="E11" t="n">
-        <v>16779</v>
+        <v>6342</v>
       </c>
       <c r="F11" t="n">
-        <v>1108</v>
+        <v>78</v>
       </c>
       <c r="G11" t="n">
-        <v>31.51</v>
+        <v>21.97</v>
       </c>
       <c r="H11" t="n">
-        <v>48.49</v>
+        <v>6.31</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -727,31 +757,135 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>An error occurred. ... ValueError('Unable to extract date from table header.')</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Texas -- Bexar County</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>43992</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1805</v>
+      </c>
+      <c r="D13" t="n">
+        <v>54</v>
+      </c>
+      <c r="E13" t="n">
+        <v>280</v>
+      </c>
+      <c r="F13" t="n">
+        <v>17</v>
+      </c>
+      <c r="G13" t="n">
+        <v>15.51</v>
+      </c>
+      <c r="H13" t="n">
+        <v>31.48</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>Virginia</t>
         </is>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>An error occurred. ... URLError(TimeoutError(10060, 'A connection attempt failed because the connected party did not properly respond after a period of time, or established connection failed because connected host has failed to respond', None, 10060, None))</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Washington, DC</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="n">
         <v>43991</v>
       </c>
-      <c r="C12" t="n">
-        <v>51738</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1496</v>
-      </c>
-      <c r="E12" t="n">
-        <v>7154</v>
-      </c>
-      <c r="F12" t="n">
-        <v>311</v>
-      </c>
-      <c r="G12" t="n">
-        <v>13.83</v>
-      </c>
-      <c r="H12" t="n">
-        <v>20.79</v>
-      </c>
-      <c r="I12" t="inlineStr">
+      <c r="C15" t="n">
+        <v>9474</v>
+      </c>
+      <c r="D15" t="n">
+        <v>495</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4331</v>
+      </c>
+      <c r="F15" t="n">
+        <v>367</v>
+      </c>
+      <c r="G15" t="n">
+        <v>45.71</v>
+      </c>
+      <c r="H15" t="n">
+        <v>74.14</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Wisconsin -- Milwaukee</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>43992</v>
+      </c>
+      <c r="C16" t="n">
+        <v>9161</v>
+      </c>
+      <c r="D16" t="n">
+        <v>306</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2597</v>
+      </c>
+      <c r="F16" t="n">
+        <v>129</v>
+      </c>
+      <c r="G16" t="n">
+        <v>28.35</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>Success!</t>
         </is>

</xml_diff>